<commit_message>
made some neatness twesaks
</commit_message>
<xml_diff>
--- a/Artificial Dataset Metadata.xlsx
+++ b/Artificial Dataset Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jon/Documents/Projects/SDS Workshop Projects/SDS Slack Challenge 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F28F702-379D-1346-97C3-EAAC222827A1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8C24B-6941-4B4B-9C46-C26E4B969D17}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>